<commit_message>
Excel con propiedad de simetria de informacion mutua
</commit_message>
<xml_diff>
--- a/parte_2.xlsx
+++ b/parte_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\Facultad\3er Ano\2do cuatri\teoria de la info\TP teoria de la info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{00453BA4-67CE-4E62-A7D9-BEAFC7F6BDC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E1FC841-44B8-4D0F-86A8-BDE38224C17E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="canal1 guia" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="74">
   <si>
     <t>Probabilidad</t>
   </si>
@@ -253,6 +253,12 @@
   <si>
     <t>S6</t>
   </si>
+  <si>
+    <t>I(B,A) =</t>
+  </si>
+  <si>
+    <t>Propiedad de simetria de informacion mutua</t>
+  </si>
 </sst>
 </file>
 
@@ -323,7 +329,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="63">
+  <borders count="69">
     <border>
       <left/>
       <right/>
@@ -1153,11 +1159,77 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="141">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1386,6 +1458,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="67" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="66" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="63" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="65" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="64" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -12968,8 +13053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C4555A7-6498-4EEB-8A3F-7230C1163FEF}">
   <dimension ref="B1:S109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+    <sheetView topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="L92" sqref="L92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14186,6 +14271,26 @@
       </c>
     </row>
     <row r="87" spans="2:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="89" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="90" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H90" s="138" t="s">
+        <v>73</v>
+      </c>
+      <c r="I90" s="139"/>
+      <c r="J90" s="139"/>
+      <c r="K90" s="140"/>
+    </row>
+    <row r="91" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H91" s="137" t="s">
+        <v>72</v>
+      </c>
+      <c r="I91" s="136">
+        <f>J98-P103</f>
+        <v>1.7020567101001527E-2</v>
+      </c>
+      <c r="J91" s="134"/>
+      <c r="K91" s="135"/>
+    </row>
     <row r="92" spans="2:19" x14ac:dyDescent="0.25">
       <c r="G92" s="100" t="s">
         <v>60</v>
@@ -14497,9 +14602,10 @@
     </row>
     <row r="109" spans="2:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="35">
+  <mergeCells count="36">
     <mergeCell ref="F1:J3"/>
     <mergeCell ref="K31:O31"/>
+    <mergeCell ref="H90:K90"/>
     <mergeCell ref="B77:C77"/>
     <mergeCell ref="B78:C78"/>
     <mergeCell ref="B79:C79"/>
@@ -14545,8 +14651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56D1FF4C-86CD-4A5B-AD25-94E64184D5A5}">
   <dimension ref="B1:X106"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B78" sqref="B78:C79"/>
+    <sheetView topLeftCell="B74" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L90" sqref="L90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15812,6 +15918,26 @@
       </c>
     </row>
     <row r="84" spans="2:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="86" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="87" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H87" s="138" t="s">
+        <v>73</v>
+      </c>
+      <c r="I87" s="139"/>
+      <c r="J87" s="139"/>
+      <c r="K87" s="140"/>
+    </row>
+    <row r="88" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H88" s="137" t="s">
+        <v>72</v>
+      </c>
+      <c r="I88" s="136">
+        <f>J95-P100</f>
+        <v>3.2936543304823207E-2</v>
+      </c>
+      <c r="J88" s="134"/>
+      <c r="K88" s="135"/>
+    </row>
     <row r="89" spans="2:19" x14ac:dyDescent="0.25">
       <c r="G89" s="100" t="s">
         <v>60</v>
@@ -16134,7 +16260,8 @@
     </row>
     <row r="106" spans="2:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="36">
+  <mergeCells count="37">
+    <mergeCell ref="H87:K87"/>
     <mergeCell ref="F1:J3"/>
     <mergeCell ref="G15:J16"/>
     <mergeCell ref="G27:J28"/>
@@ -16183,8 +16310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49BC2625-C4A5-41A8-9B4F-26728C066F48}">
   <dimension ref="B1:S112"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F95" sqref="F95"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="L105" sqref="L105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17779,6 +17906,26 @@
       </c>
     </row>
     <row r="90" spans="2:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="92" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="93" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H93" s="138" t="s">
+        <v>73</v>
+      </c>
+      <c r="I93" s="139"/>
+      <c r="J93" s="139"/>
+      <c r="K93" s="140"/>
+    </row>
+    <row r="94" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H94" s="137" t="s">
+        <v>72</v>
+      </c>
+      <c r="I94" s="136">
+        <f>J101-P109</f>
+        <v>3.1285438630455964E-2</v>
+      </c>
+      <c r="J94" s="134"/>
+      <c r="K94" s="135"/>
+    </row>
     <row r="95" spans="2:17" x14ac:dyDescent="0.25">
       <c r="G95" s="100" t="s">
         <v>60</v>
@@ -18180,8 +18327,9 @@
     </row>
     <row r="112" spans="2:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="36">
+  <mergeCells count="37">
     <mergeCell ref="G28:J29"/>
+    <mergeCell ref="H93:K93"/>
     <mergeCell ref="F1:J3"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="G16:J17"/>

</xml_diff>